<commit_message>
a whole buttload of models to test
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN06/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN06/best_accuracy_series.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:Q2"/>
+  <dimension ref="B1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,55 +502,87 @@
           <t>epoch800</t>
         </is>
       </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>epoch850</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>epoch900</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>epoch950</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>epoch1000</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="C2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="D2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="E2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="F2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="G2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="H2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="I2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="J2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="K2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="L2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="M2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="N2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="O2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="P2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
       </c>
       <c r="Q2" t="n">
-        <v>79.55729141831398</v>
+        <v>78.38541641831398</v>
+      </c>
+      <c r="R2" t="n">
+        <v>78.38541641831398</v>
+      </c>
+      <c r="S2" t="n">
+        <v>78.38541641831398</v>
+      </c>
+      <c r="T2" t="n">
+        <v>78.38541641831398</v>
+      </c>
+      <c r="U2" t="n">
+        <v>78.38541641831398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>